<commit_message>
Update to cost calculators
</commit_message>
<xml_diff>
--- a/CBI-CS_Cost_Calculator.xlsx
+++ b/CBI-CS_Cost_Calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pkelley/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0B1C2E-8F43-EB4C-983F-3BCCC3F7CF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097FA4C5-9871-7A47-811F-3172B468D30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12740" yWindow="-21240" windowWidth="27280" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8980" yWindow="-18380" windowWidth="23300" windowHeight="17020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burnout Cost Calculator" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Burnout Cost Factors</t>
   </si>
   <si>
-    <t>Value</t>
+    <t>Inputs</t>
   </si>
   <si>
     <t>Number of Employees</t>
@@ -62,30 +62,79 @@
     <t>Average Mental Health Claim per Employee ($)</t>
   </si>
   <si>
+    <t>Manager Time Lost to Burnout Issues (hrs/month)</t>
+  </si>
+  <si>
+    <t>Average Manager Hourly Rate ($)</t>
+  </si>
+  <si>
+    <t>Opportunity Cost (Missed Revenue or Projects $)</t>
+  </si>
+  <si>
+    <t>Presenteeism Cost Factor (as % of Salary)</t>
+  </si>
+  <si>
+    <t>Burnout Reduction Target (%)</t>
+  </si>
+  <si>
     <t>Calculated Costs</t>
   </si>
   <si>
+    <t>Results</t>
+  </si>
+  <si>
     <t>Turnover Cost ($)</t>
   </si>
   <si>
-    <t>Turnover Cost Due to Burnout ($)</t>
-  </si>
-  <si>
     <t>Productivity Loss Cost Due to Burnout ($)</t>
+  </si>
+  <si>
+    <t>Sick Leave Cost ($)</t>
+  </si>
+  <si>
+    <t>Mental Health Claim Cost ($)</t>
+  </si>
+  <si>
+    <t>Manager Time Cost ($)</t>
+  </si>
+  <si>
+    <t>Presenteeism Cost ($)</t>
+  </si>
+  <si>
+    <t>Opportunity Cost ($)</t>
+  </si>
+  <si>
+    <t>Total Burnout Cost ($)</t>
+  </si>
+  <si>
+    <t>Projected Savings if Burnout Reduced ($)</t>
+  </si>
+  <si>
+    <t>Cost per Employee ($)</t>
+  </si>
+  <si>
+    <t>% Payroll Lost to Burnout</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\$#,##0"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,7 +148,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,7 +157,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD7E4BC"/>
+        <fgColor rgb="FF4472C4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -140,17 +195,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,16 +506,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="45.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -479,91 +530,183 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5">
-        <v>200</v>
-      </c>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4">
-        <v>0.1</v>
-      </c>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3">
-        <v>120000</v>
-      </c>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4">
-        <v>0.2</v>
-      </c>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5">
-        <v>5</v>
-      </c>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3">
-        <v>2000</v>
-      </c>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3">
-        <f>B3*B2*B4</f>
-        <v>2400000</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="6">
-        <f>B2*B3*B4*B5</f>
-        <v>2400000</v>
-      </c>
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6">
-        <f>B2*B4*B6</f>
-        <v>4800000</v>
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="4">
+        <f>(B3*B4)*(B2/100)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="4">
+        <f>B3*B2*(B5/100)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="4">
+        <f>B2*B6*(B4/260)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="4">
+        <f>B2*B7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="4">
+        <f>B8*B9*12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="4">
+        <f>B3*B2*(B11/100)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="4">
+        <f>B10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="4">
+        <f>SUM(B16:B22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="4">
+        <f>B23*(B12/100)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="4" t="e">
+        <f>B23/B2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="5" t="e">
+        <f>B23/(B3*B4)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>